<commit_message>
feat: Update scores sheet
</commit_message>
<xml_diff>
--- a/data/raw/scores.xlsx
+++ b/data/raw/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/gitsky/hatespeech/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD05ECC4-0237-024C-9E68-EF88C1DC9A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4843D4-5F19-C94B-88C8-BABD783A87D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19660" xr2:uid="{E424606D-9CEA-BC47-9A9F-F74680F194A3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>Model</t>
   </si>
@@ -83,6 +83,39 @@
   </si>
   <si>
     <t>ELECTRA-3rd-iteration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - contains_offensive_word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - is_all_caps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - contains_positive_swear_word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - is_dr_answer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - has_been_moderated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - is_spam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - is_mention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - use_danlp_model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - use_attack_model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - use_tfidf_model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    - has_positive_sentiment</t>
   </si>
 </sst>
 </file>
@@ -616,15 +649,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE797D34-3AFC-3E45-A478-B30E4E8DD871}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
@@ -809,93 +842,214 @@
     </row>
     <row r="9" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3">
-        <v>0.42230000000000001</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.87</v>
-      </c>
-      <c r="D9" s="5">
-        <v>0.56859999999999999</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.43690000000000001</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0.84909999999999997</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0.57689999999999997</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3">
-        <v>0.15049999999999999</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.1802</v>
-      </c>
-      <c r="D10" s="5">
-        <v>0.16400000000000001</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.1699</v>
-      </c>
-      <c r="F10" s="4">
-        <v>0.19439999999999999</v>
-      </c>
-      <c r="G10" s="5">
-        <v>0.18129999999999999</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="7"/>
+    </row>
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="7"/>
+    </row>
+    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.42230000000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.87</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.56859999999999999</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.43690000000000001</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.84909999999999997</v>
+      </c>
+      <c r="G20" s="5">
+        <v>0.57689999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.15049999999999999</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.1802</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.1699</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.19439999999999999</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.18129999999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B22" s="3">
         <v>0.52910000000000001</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C22" s="4">
         <v>0.9083</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D22" s="5">
         <v>0.66869999999999996</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E22" s="3">
         <v>0.57279999999999998</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F22" s="4">
         <v>0.92190000000000005</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G22" s="5">
         <v>0.70660000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B23" s="8">
         <v>0.48060000000000003</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C23" s="9">
         <v>1</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D23" s="10">
         <v>0.6492</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E23" s="8">
         <v>0.58250000000000002</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F23" s="9">
         <v>0.99170000000000003</v>
       </c>
-      <c r="G12" s="10">
+      <c r="G23" s="10">
         <v>0.7339</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: Update score sheet
</commit_message>
<xml_diff>
--- a/data/raw/scores.xlsx
+++ b/data/raw/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/gitsky/hatespeech/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E4843D4-5F19-C94B-88C8-BABD783A87D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A186A1-B3D9-2242-8239-6A74E3563BFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19660" xr2:uid="{E424606D-9CEA-BC47-9A9F-F74680F194A3}"/>
   </bookViews>
@@ -652,7 +652,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -844,122 +844,206 @@
       <c r="A9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="7"/>
+      <c r="B9" s="3">
+        <v>0.88349999999999995</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.88780000000000003</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.88560000000000005</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0.86919999999999997</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="7"/>
+      <c r="B10" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.87260000000000004</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.82220000000000004</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.85850000000000004</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="7"/>
+      <c r="B11" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.87260000000000004</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.88519999999999999</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.82220000000000004</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0.85850000000000004</v>
+      </c>
     </row>
     <row r="12" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
+      <c r="B12" s="3">
+        <v>0.89319999999999999</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.87619999999999998</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.88460000000000005</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.90290000000000004</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.82669999999999999</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.86309999999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="7"/>
+      <c r="B13" s="3">
+        <v>0.88829999999999998</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.88829999999999998</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.88829999999999998</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.84470000000000001</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.87060000000000004</v>
+      </c>
     </row>
     <row r="14" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="6"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="3"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="7"/>
+      <c r="B15" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.87890000000000001</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="G15" s="5">
+        <v>0.85780000000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="6"/>
+      <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="3"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="7"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="6"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="3"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="7"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="3"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="7"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="7"/>
+      <c r="B19" s="3">
+        <v>0.91259999999999997</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.83560000000000001</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.87239999999999995</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.93200000000000005</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.79669999999999996</v>
+      </c>
+      <c r="G19" s="5">
+        <v>0.85909999999999997</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">

</xml_diff>

<commit_message>
feat: Add a few comments to the score sheet
</commit_message>
<xml_diff>
--- a/data/raw/scores.xlsx
+++ b/data/raw/scores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/gitsky/hatespeech/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F2F690-09C6-3543-8FA6-20C84752DF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31590E18-3189-1943-93A4-DCCE69E2D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19660" xr2:uid="{E424606D-9CEA-BC47-9A9F-F74680F194A3}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Model</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t xml:space="preserve">    - has_positive_sentiment</t>
+  </si>
+  <si>
+    <t>&lt;-- Catches comments that the others don't (since recall is lower), but also contributes to a decrease in precision. Label function can only mark OFFENSIVE and ABSTAIN.</t>
+  </si>
+  <si>
+    <t>&lt;-- Significantly increases precision, while reducing recall, which is probably because this LF can mark things as NOT_OFFENSIVE as well as the other two.</t>
   </si>
 </sst>
 </file>
@@ -660,7 +666,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,7 +678,7 @@
     <col min="5" max="5" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="143.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
@@ -1033,8 +1039,11 @@
       <c r="G16" s="5">
         <v>0.75609999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="H16" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>24</v>
       </c>
@@ -1057,7 +1066,7 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>25</v>
       </c>
@@ -1079,8 +1088,11 @@
       <c r="G18" s="7">
         <v>0.88290000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>26</v>
       </c>
@@ -1103,7 +1115,7 @@
         <v>0.85909999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>8</v>
       </c>
@@ -1126,7 +1138,7 @@
         <v>0.57689999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>9</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>0.18129999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>10</v>
       </c>
@@ -1172,7 +1184,7 @@
         <v>0.70660000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
feat: Update scores to new evaluation dataset with three annotators
</commit_message>
<xml_diff>
--- a/data/raw/scores.xlsx
+++ b/data/raw/scores.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan/gitsky/hatespeech/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31590E18-3189-1943-93A4-DCCE69E2D05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0537D9B9-53CD-854A-B64D-763D2522D52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19660" xr2:uid="{E424606D-9CEA-BC47-9A9F-F74680F194A3}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="19660" activeTab="1" xr2:uid="{E424606D-9CEA-BC47-9A9F-F74680F194A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="old-labels" sheetId="1" r:id="rId1"/>
+    <sheet name="new-labels" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="29">
   <si>
     <t>Model</t>
   </si>
@@ -46,9 +48,6 @@
     <t>Precision</t>
   </si>
   <si>
-    <t>F1-score</t>
-  </si>
-  <si>
     <t>XLMR-base-1st-iteration</t>
   </si>
   <si>
@@ -122,6 +121,9 @@
   </si>
   <si>
     <t>&lt;-- Significantly increases precision, while reducing recall, which is probably because this LF can mark things as NOT_OFFENSIVE as well as the other two.</t>
+  </si>
+  <si>
+    <t>F2-score</t>
   </si>
 </sst>
 </file>
@@ -316,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -349,6 +351,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -665,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE797D34-3AFC-3E45-A478-B30E4E8DD871}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,12 +691,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C1" s="18"/>
       <c r="D1" s="19"/>
       <c r="E1" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="19"/>
@@ -705,7 +710,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>1</v>
@@ -714,12 +719,12 @@
         <v>2</v>
       </c>
       <c r="G2" s="15" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3">
         <v>0.74760000000000004</v>
@@ -727,8 +732,9 @@
       <c r="C3" s="4">
         <v>0.82799999999999996</v>
       </c>
-      <c r="D3" s="5">
-        <v>0.78569999999999995</v>
+      <c r="D3" s="24">
+        <f>5*B3*C3/((4*C3)+B3)</f>
+        <v>0.762406148389004</v>
       </c>
       <c r="E3" s="3">
         <v>0.76700000000000002</v>
@@ -736,13 +742,14 @@
       <c r="F3" s="4">
         <v>0.84040000000000004</v>
       </c>
-      <c r="G3" s="5">
-        <v>0.80200000000000005</v>
+      <c r="G3" s="24">
+        <f>5*E3*F3/((4*F3)+E3)</f>
+        <v>0.78063605096158495</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>0.88349999999999995</v>
@@ -751,7 +758,8 @@
         <v>0.83489999999999998</v>
       </c>
       <c r="D4" s="5">
-        <v>0.85850000000000004</v>
+        <f t="shared" ref="D4:D23" si="0">5*B4*C4/((4*C4)+B4)</f>
+        <v>0.87333256375648216</v>
       </c>
       <c r="E4" s="3">
         <v>0.91749999999999998</v>
@@ -760,12 +768,13 @@
         <v>0.80769999999999997</v>
       </c>
       <c r="G4" s="5">
-        <v>0.85909999999999997</v>
+        <f t="shared" ref="G4:G23" si="1">5*E4*F4/((4*F4)+E4)</f>
+        <v>0.89321499168334029</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3">
         <v>0.89319999999999999</v>
@@ -773,8 +782,9 @@
       <c r="C5" s="4">
         <v>0.90639999999999998</v>
       </c>
-      <c r="D5" s="7">
-        <v>0.89980000000000004</v>
+      <c r="D5" s="5">
+        <f t="shared" si="0"/>
+        <v>0.89580915287244411</v>
       </c>
       <c r="E5" s="3">
         <v>0.93200000000000005</v>
@@ -782,13 +792,14 @@
       <c r="F5" s="4">
         <v>0.83479999999999999</v>
       </c>
-      <c r="G5" s="5">
-        <v>0.88070000000000004</v>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.91079041018917395</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="3">
         <v>0.75729999999999997</v>
@@ -797,7 +808,8 @@
         <v>0.96299999999999997</v>
       </c>
       <c r="D6" s="5">
-        <v>0.8478</v>
+        <f t="shared" si="0"/>
+        <v>0.79109615342893702</v>
       </c>
       <c r="E6" s="3">
         <v>0.81069999999999998</v>
@@ -806,12 +818,13 @@
         <v>0.90269999999999995</v>
       </c>
       <c r="G6" s="5">
-        <v>0.85419999999999996</v>
+        <f t="shared" si="1"/>
+        <v>0.82756857401334383</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3">
         <v>0.87380000000000002</v>
@@ -820,7 +833,8 @@
         <v>0.82569999999999999</v>
       </c>
       <c r="D7" s="5">
-        <v>0.84909999999999997</v>
+        <f t="shared" si="0"/>
+        <v>0.8637368433654169</v>
       </c>
       <c r="E7" s="3">
         <v>0.89319999999999999</v>
@@ -829,12 +843,13 @@
         <v>0.81059999999999999</v>
       </c>
       <c r="G7" s="5">
-        <v>0.84989999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.87536018957345962</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="3">
         <v>0.89810000000000001</v>
@@ -843,7 +858,8 @@
         <v>0.89370000000000005</v>
       </c>
       <c r="D8" s="5">
-        <v>0.89590000000000003</v>
+        <f t="shared" si="0"/>
+        <v>0.89721653736949181</v>
       </c>
       <c r="E8" s="3">
         <v>0.91259999999999997</v>
@@ -851,13 +867,14 @@
       <c r="F8" s="4">
         <v>0.85450000000000004</v>
       </c>
-      <c r="G8" s="7">
-        <v>0.88260000000000005</v>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.90035641712464776</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="3">
         <v>0.88349999999999995</v>
@@ -866,7 +883,8 @@
         <v>0.88780000000000003</v>
       </c>
       <c r="D9" s="5">
-        <v>0.88560000000000005</v>
+        <f t="shared" si="0"/>
+        <v>0.88435666448688732</v>
       </c>
       <c r="E9" s="3">
         <v>0.90290000000000004</v>
@@ -875,12 +893,13 @@
         <v>0.83779999999999999</v>
       </c>
       <c r="G9" s="5">
-        <v>0.86919999999999997</v>
+        <f t="shared" si="1"/>
+        <v>0.88908302578688791</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="3">
         <v>0.89810000000000001</v>
@@ -889,7 +908,8 @@
         <v>0.87260000000000004</v>
       </c>
       <c r="D10" s="5">
-        <v>0.88519999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.89288146291443538</v>
       </c>
       <c r="E10" s="3">
         <v>0.89810000000000001</v>
@@ -898,12 +918,13 @@
         <v>0.82220000000000004</v>
       </c>
       <c r="G10" s="5">
-        <v>0.85850000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0.88181926962669266</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="3">
         <v>0.88349999999999995</v>
@@ -912,7 +933,8 @@
         <v>0.89659999999999995</v>
       </c>
       <c r="D11" s="5">
-        <v>0.89</v>
+        <f t="shared" si="0"/>
+        <v>0.88608928611378324</v>
       </c>
       <c r="E11" s="3">
         <v>0.88349999999999995</v>
@@ -921,13 +943,14 @@
         <v>0.84650000000000003</v>
       </c>
       <c r="G11" s="5">
-        <v>0.86460000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0.87584348284342428</v>
       </c>
       <c r="H11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="3">
         <v>0.89319999999999999</v>
@@ -936,7 +959,8 @@
         <v>0.87619999999999998</v>
       </c>
       <c r="D12" s="5">
-        <v>0.88460000000000005</v>
+        <f t="shared" si="0"/>
+        <v>0.88974743065029571</v>
       </c>
       <c r="E12" s="3">
         <v>0.90290000000000004</v>
@@ -945,12 +969,13 @@
         <v>0.82669999999999999</v>
       </c>
       <c r="G12" s="5">
-        <v>0.86309999999999998</v>
+        <f t="shared" si="1"/>
+        <v>0.88655655984987058</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3">
         <v>0.88829999999999998</v>
@@ -959,6 +984,7 @@
         <v>0.88829999999999998</v>
       </c>
       <c r="D13" s="5">
+        <f t="shared" si="0"/>
         <v>0.88829999999999998</v>
       </c>
       <c r="E13" s="3">
@@ -968,12 +994,13 @@
         <v>0.84470000000000001</v>
       </c>
       <c r="G13" s="5">
-        <v>0.87060000000000004</v>
+        <f t="shared" si="1"/>
+        <v>0.886886611798265</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="3">
         <v>0.88829999999999998</v>
@@ -982,7 +1009,8 @@
         <v>0.85119999999999996</v>
       </c>
       <c r="D14" s="5">
-        <v>0.86939999999999995</v>
+        <f t="shared" si="0"/>
+        <v>0.8806235121473992</v>
       </c>
       <c r="E14" s="3">
         <v>0.90290000000000004</v>
@@ -991,12 +1019,13 @@
         <v>0.83779999999999999</v>
       </c>
       <c r="G14" s="5">
-        <v>0.86919999999999997</v>
+        <f t="shared" si="1"/>
+        <v>0.88908302578688791</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3">
         <v>0.89810000000000001</v>
@@ -1005,7 +1034,8 @@
         <v>0.86050000000000004</v>
       </c>
       <c r="D15" s="5">
-        <v>0.87890000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.89031940508283203</v>
       </c>
       <c r="E15" s="3">
         <v>0.90780000000000005</v>
@@ -1014,12 +1044,13 @@
         <v>0.81299999999999994</v>
       </c>
       <c r="G15" s="5">
-        <v>0.85780000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.88711163998269149</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="6">
         <v>0.98060000000000003</v>
@@ -1027,8 +1058,9 @@
       <c r="C16" s="4">
         <v>0.68469999999999998</v>
       </c>
-      <c r="D16" s="5">
-        <v>0.80640000000000001</v>
+      <c r="D16" s="7">
+        <f t="shared" si="0"/>
+        <v>0.90258754100123684</v>
       </c>
       <c r="E16" s="6">
         <v>0.97089999999999999</v>
@@ -1037,15 +1069,16 @@
         <v>0.61919999999999997</v>
       </c>
       <c r="G16" s="5">
-        <v>0.75609999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.87185845636221249</v>
       </c>
       <c r="H16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3">
         <v>0.85919999999999996</v>
@@ -1054,7 +1087,8 @@
         <v>0.88060000000000005</v>
       </c>
       <c r="D17" s="5">
-        <v>0.86980000000000002</v>
+        <f t="shared" si="0"/>
+        <v>0.86339638488223458</v>
       </c>
       <c r="E17" s="3">
         <v>0.89319999999999999</v>
@@ -1063,12 +1097,13 @@
         <v>0.84789999999999999</v>
       </c>
       <c r="G17" s="5">
-        <v>0.87</v>
+        <f t="shared" si="1"/>
+        <v>0.88375686146377908</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3">
         <v>0.88829999999999998</v>
@@ -1077,7 +1112,8 @@
         <v>0.95309999999999995</v>
       </c>
       <c r="D18" s="5">
-        <v>0.91959999999999997</v>
+        <f t="shared" si="0"/>
+        <v>0.90054537622056297</v>
       </c>
       <c r="E18" s="3">
         <v>0.87860000000000005</v>
@@ -1085,16 +1121,17 @@
       <c r="F18" s="4">
         <v>0.88729999999999998</v>
       </c>
-      <c r="G18" s="7">
-        <v>0.88290000000000002</v>
+      <c r="G18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88032632458557314</v>
       </c>
       <c r="H18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="3">
         <v>0.91259999999999997</v>
@@ -1103,7 +1140,8 @@
         <v>0.83560000000000001</v>
       </c>
       <c r="D19" s="5">
-        <v>0.87239999999999995</v>
+        <f t="shared" si="0"/>
+        <v>0.89608526439482961</v>
       </c>
       <c r="E19" s="3">
         <v>0.93200000000000005</v>
@@ -1112,12 +1150,13 @@
         <v>0.79669999999999996</v>
       </c>
       <c r="G19" s="5">
-        <v>0.85909999999999997</v>
+        <f t="shared" si="1"/>
+        <v>0.90138438380110708</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" s="3">
         <v>0.42230000000000001</v>
@@ -1126,7 +1165,8 @@
         <v>0.87</v>
       </c>
       <c r="D20" s="5">
-        <v>0.56859999999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.47074930169387286</v>
       </c>
       <c r="E20" s="3">
         <v>0.43690000000000001</v>
@@ -1135,12 +1175,13 @@
         <v>0.84909999999999997</v>
       </c>
       <c r="G20" s="5">
-        <v>0.57689999999999997</v>
+        <f t="shared" si="1"/>
+        <v>0.48388045548222158</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B21" s="3">
         <v>0.15049999999999999</v>
@@ -1149,7 +1190,8 @@
         <v>0.1802</v>
       </c>
       <c r="D21" s="5">
-        <v>0.16400000000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.15563009296453573</v>
       </c>
       <c r="E21" s="3">
         <v>0.1699</v>
@@ -1158,12 +1200,13 @@
         <v>0.19439999999999999</v>
       </c>
       <c r="G21" s="5">
-        <v>0.18129999999999999</v>
+        <f t="shared" si="1"/>
+        <v>0.17429319261213719</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="3">
         <v>0.52910000000000001</v>
@@ -1172,7 +1215,8 @@
         <v>0.9083</v>
       </c>
       <c r="D22" s="5">
-        <v>0.66869999999999996</v>
+        <f t="shared" si="0"/>
+        <v>0.57730284938615661</v>
       </c>
       <c r="E22" s="3">
         <v>0.57279999999999998</v>
@@ -1181,12 +1225,13 @@
         <v>0.92190000000000005</v>
       </c>
       <c r="G22" s="5">
-        <v>0.70660000000000001</v>
+        <f t="shared" si="1"/>
+        <v>0.61973561167965441</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B23" s="8">
         <v>0.48060000000000003</v>
@@ -1195,7 +1240,8 @@
         <v>1</v>
       </c>
       <c r="D23" s="10">
-        <v>0.6492</v>
+        <f t="shared" si="0"/>
+        <v>0.53631210105789406</v>
       </c>
       <c r="E23" s="8">
         <v>0.58250000000000002</v>
@@ -1204,7 +1250,8 @@
         <v>0.99170000000000003</v>
       </c>
       <c r="G23" s="10">
-        <v>0.7339</v>
+        <f t="shared" si="1"/>
+        <v>0.63489465412261215</v>
       </c>
     </row>
   </sheetData>
@@ -1216,4 +1263,598 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6100B315-A36D-A44B-93E6-B7B0C5F75464}">
+  <dimension ref="A1:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="143.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="18"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A2" s="21"/>
+      <c r="B2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="22">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.7944</v>
+      </c>
+      <c r="D3" s="24">
+        <f>5*B3*C3/((4*C3)+B3)</f>
+        <v>0.78846895020935281</v>
+      </c>
+      <c r="E3" s="22">
+        <v>0.72560000000000002</v>
+      </c>
+      <c r="F3" s="23">
+        <v>0.72560000000000002</v>
+      </c>
+      <c r="G3" s="24">
+        <f t="shared" ref="G3:G23" si="0">5*E3*F3/((4*F3)+E3)</f>
+        <v>0.72560000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C4" s="4">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" ref="D4:D23" si="1">5*B4*C4/((4*C4)+B4)</f>
+        <v>0.87069988256165498</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.70330000000000004</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84729224003021963</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.91669999999999996</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.80820000000000003</v>
+      </c>
+      <c r="D5" s="7">
+        <f t="shared" si="1"/>
+        <v>0.89273037715387393</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.89770000000000005</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0.74809999999999999</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.86317751471684534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.81020000000000003</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.85780000000000001</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="1"/>
+        <v>0.81929263922289808</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.73950000000000005</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.8196</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>0.7542425147465095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.88890000000000002</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.7742</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.8633193416463858</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.87909999999999999</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>0.83630507461063841</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.90739999999999998</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.82010000000000005</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88848409666173167</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0.74129999999999996</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>0.85788826395728568</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.81859999999999999</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88098820850808857</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0.73729999999999996</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84304728528088702</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.79420000000000002</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87170196300027025</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.85482559664306323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.87960000000000005</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.86677302916546362</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.87909999999999999</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84984274702895002</v>
+      </c>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.80830000000000002</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87857844988260347</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.88370000000000004</v>
+      </c>
+      <c r="F12" s="4">
+        <v>0.71699999999999997</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.8444343897433163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.81510000000000005</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88017471444030304</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.87909999999999999</v>
+      </c>
+      <c r="F13" s="4">
+        <v>0.747</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84906997491660419</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.89349999999999996</v>
+      </c>
+      <c r="C14" s="4">
+        <v>0.80079999999999996</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87328190982986287</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.88839999999999997</v>
+      </c>
+      <c r="F14" s="4">
+        <v>0.72619999999999996</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.85041136771064019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.86570000000000003</v>
+      </c>
+      <c r="C15" s="4">
+        <v>0.79910000000000003</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.8515064498658329</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.87439999999999996</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0.74309999999999998</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84455474680253717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="3">
+        <v>0.97219999999999995</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="1"/>
+        <v>0.8501718064396514</v>
+      </c>
+      <c r="E16" s="6">
+        <v>0.97670000000000001</v>
+      </c>
+      <c r="F16" s="4">
+        <v>0.54969999999999997</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84536606833569505</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="3">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="C17" s="4">
+        <v>0.81969999999999998</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.87057806682520233</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.86980000000000002</v>
+      </c>
+      <c r="F17" s="4">
+        <v>0.73909999999999998</v>
+      </c>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84008831216350432</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3">
+        <v>0.89810000000000001</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.85840000000000005</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88986891982362581</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.86050000000000004</v>
+      </c>
+      <c r="F18" s="4">
+        <v>0.80789999999999995</v>
+      </c>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84943910217247864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A19" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="6">
+        <v>0.93520000000000003</v>
+      </c>
+      <c r="C19" s="4">
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.89144114958870724</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.90229999999999999</v>
+      </c>
+      <c r="F19" s="4">
+        <v>0.68310000000000004</v>
+      </c>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.84788446089085756</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="3">
+        <v>0.42130000000000001</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.80530000000000002</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="1"/>
+        <v>0.46571433081674679</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.4279</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.75409999999999999</v>
+      </c>
+      <c r="G20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.46842520976686119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="3">
+        <v>0.17130000000000001</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.17699999999999999</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="1"/>
+        <v>0.17241044012282497</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.15809999999999999</v>
+      </c>
+      <c r="F21" s="4">
+        <v>0.15379999999999999</v>
+      </c>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.15722087158929263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="3">
+        <v>0.53239999999999998</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.88460000000000005</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.57846251351085776</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.56279999999999997</v>
+      </c>
+      <c r="F22" s="4">
+        <v>0.86429999999999996</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.60501000000000005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="8">
+        <v>0.55089999999999995</v>
+      </c>
+      <c r="C23" s="9">
+        <v>0.97540000000000004</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" si="1"/>
+        <v>0.60342263896687243</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.97319999999999995</v>
+      </c>
+      <c r="G23" s="10">
+        <f t="shared" si="0"/>
+        <v>0.56072139642711027</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>